<commit_message>
changed strain 1452 to G418 in 1660
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_1660.xlsx
+++ b/bioSample/bioSample_1660.xlsx
@@ -88,6 +88,9 @@
     <t xml:space="preserve">CNAG_02566</t>
   </si>
   <si>
+    <t xml:space="preserve">G418</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDY1442</t>
   </si>
   <si>
@@ -98,9 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">CNAG_04864.CNAG_02566</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G418</t>
   </si>
   <si>
     <t xml:space="preserve">TDY1662</t>
@@ -127,6 +127,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -211,7 +212,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,10 +556,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>16</v>
@@ -587,10 +588,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>16</v>
@@ -619,10 +620,10 @@
         <v>13</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>16</v>
@@ -651,10 +652,10 @@
         <v>13</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>16</v>
@@ -669,7 +670,7 @@
         <v>19</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,10 +687,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>16</v>
@@ -704,7 +705,7 @@
         <v>19</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,10 +722,10 @@
         <v>13</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>16</v>
@@ -739,7 +740,7 @@
         <v>19</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,7 +775,7 @@
         <v>19</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,7 +810,7 @@
         <v>19</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +880,7 @@
         <v>19</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,7 +950,7 @@
         <v>19</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>